<commit_message>
updated caption on hardware overview image
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Battery 1</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>sum</t>
   </si>
 </sst>
 </file>
@@ -141,10 +150,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -428,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B24" sqref="B24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,35 +451,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
+      <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B3">
@@ -489,7 +498,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4">
@@ -508,7 +517,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5">
@@ -527,7 +536,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6">
@@ -546,7 +555,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B7">
@@ -565,7 +574,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8">
@@ -584,7 +593,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B9">
@@ -603,7 +612,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10">
@@ -622,7 +631,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11">
@@ -641,7 +650,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12">
@@ -660,7 +669,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13">
@@ -679,7 +688,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14">
@@ -698,7 +707,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B15">
@@ -717,7 +726,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16">
@@ -736,7 +745,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B17">
@@ -755,7 +764,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B18">
@@ -774,7 +783,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B19">
@@ -793,7 +802,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B20">
@@ -812,7 +821,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21">
@@ -830,6 +839,45 @@
       <c r="E21">
         <f t="shared" si="2"/>
         <v>0.2810847550927778</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <f>MIN(B3:B20)</f>
+        <v>12.29</v>
+      </c>
+      <c r="C22">
+        <f>MIN(C3:C20)</f>
+        <v>12.28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <f>MAX(B3:B20)</f>
+        <v>12.63</v>
+      </c>
+      <c r="C23">
+        <f>MAX(C3:C20)</f>
+        <v>12.56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <f>SUM(B3:B20)</f>
+        <v>225.14000000000001</v>
+      </c>
+      <c r="C24">
+        <f>SUM(C3:C20)</f>
+        <v>224.51000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>